<commit_message>
Fixing highlight at xlsx file
</commit_message>
<xml_diff>
--- a/modeling_system/trying_to_get_better.xlsx
+++ b/modeling_system/trying_to_get_better.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\01_Learning\07_Master\01_primer_semestre\modeling_and_simulation_1\programmin_opt_methods\modeling_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5783038-22D1-4C83-8435-34C4D70307EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7FE1E9-6732-4F8B-B37F-B9DA3CF6EB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -277,9 +277,6 @@
     <t>[-1.48334537e+00,  6.45004878e-01, -7.08807073e-02,  8.62231787e-04, -4.32689192e-03,  9.02570285e-02]</t>
   </si>
   <si>
-    <t>[-1.50501741,  0.68417633, -0.08906884,  0.00452517, -0.01217004, 0.09573596]</t>
-  </si>
-  <si>
     <t>I guess this is the best 3rd order model I can achieve</t>
   </si>
   <si>
@@ -379,7 +376,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">[-1.48334537e+00,  6.45004878e-01, -7.08807073e-02,  8.62231787e-04, -4.32689192e-03,  9.02570285e-02] </t>
+      <t xml:space="preserve">[-1.57757773,  0.68867778,  0.04108867, -0.07366942,  0.00197729, -0.0049589 ,  0.08804496, -0.00827193] </t>
     </r>
     <r>
       <rPr>
@@ -394,7 +391,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">[-1.57757773,  0.68867778,  0.04108867, -0.07366942,  0.00197729, -0.0049589 ,  0.08804496, -0.00827193] </t>
+      <t xml:space="preserve">[-1.50501741,  0.68417633, -0.08906884,  0.00452517, -0.01217004, 0.09573596] </t>
     </r>
     <r>
       <rPr>
@@ -523,8 +520,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -532,8 +529,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>4</v>
@@ -1303,9 +1300,9 @@
         <v>2</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I12" s="14">
+        <v>76</v>
+      </c>
+      <c r="I12" s="11">
         <v>1.9196200277646399E-2</v>
       </c>
       <c r="J12" s="10">
@@ -1410,10 +1407,10 @@
       <c r="G15" s="5">
         <v>3</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I15" s="14">
+      <c r="H15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="11">
         <v>2.3460846365785701E-2</v>
       </c>
       <c r="J15" s="10">
@@ -1446,8 +1443,8 @@
       <c r="G16" s="5">
         <v>4</v>
       </c>
-      <c r="H16" s="5" t="s">
-        <v>67</v>
+      <c r="H16" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="I16" s="10">
         <v>1.1261041047572499E-2</v>
@@ -1456,7 +1453,7 @@
         <v>1.03511575669834</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1573,7 +1570,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>61</v>
@@ -1582,7 +1579,7 @@
         <v>1E-3</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F20" s="5">
         <v>100</v>
@@ -1591,16 +1588,16 @@
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="14">
+        <v>79</v>
+      </c>
+      <c r="I20" s="11">
         <v>1.0635255409829399E-2</v>
       </c>
       <c r="J20" s="10">
         <v>1.0271734113490001</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -1609,7 +1606,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>64</v>
@@ -1618,25 +1615,25 @@
         <v>1E-3</v>
       </c>
       <c r="E21" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="G21" s="5">
         <v>4</v>
       </c>
       <c r="H21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K21" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1666,7 +1663,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1681,7 +1678,7 @@
     <row r="25" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="2"/>
@@ -1695,9 +1692,9 @@
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="11"/>
+        <v>78</v>
+      </c>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" s="2"/>

</xml_diff>

<commit_message>
Refactoring and removing mean from data, this improves a little the result of modeling
</commit_message>
<xml_diff>
--- a/modeling_system/trying_to_get_better.xlsx
+++ b/modeling_system/trying_to_get_better.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\01_Learning\07_Master\01_primer_semestre\modeling_and_simulation_1\programmin_opt_methods\modeling_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7FE1E9-6732-4F8B-B37F-B9DA3CF6EB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADBF62F-3A0F-4B1E-8FB7-6237E74D92FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -319,21 +319,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">[-1.50679337,  0.57994944, -0.04300483,  0.11451339] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>+</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -403,6 +388,30 @@
       </rPr>
       <t>+</t>
     </r>
+  </si>
+  <si>
+    <t>[-1.50679337,  0.57994944, -0.04300483,  0.11451339]</t>
+  </si>
+  <si>
+    <r>
+      <t>[-1.52183143,  0.59761894, -0.04742432,  0.11604525]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +</t>
+    </r>
+  </si>
+  <si>
+    <t>Gets a little better</t>
+  </si>
+  <si>
+    <t>Using last solution and removing mean from the data.</t>
   </si>
 </sst>
 </file>
@@ -561,8 +570,8 @@
     <xdr:to>
       <xdr:col>48</xdr:col>
       <xdr:colOff>520895</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>69591</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>13561</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -861,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +926,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -952,7 +961,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <f>1+A2</f>
         <v>2</v>
@@ -988,9 +997,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A20" si="0">1+A3</f>
+        <f t="shared" ref="A4:A22" si="0">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1024,7 +1033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1060,7 +1069,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1096,7 +1105,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1132,7 +1141,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1168,7 +1177,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="62.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1204,7 +1213,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1240,7 +1249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1276,7 +1285,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1299,10 +1308,10 @@
       <c r="G12" s="5">
         <v>2</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="11">
+      <c r="H12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="10">
         <v>1.9196200277646399E-2</v>
       </c>
       <c r="J12" s="10">
@@ -1312,52 +1321,50 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="D13" s="5">
         <v>1E-3</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="F13" s="5">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="G13" s="5">
-        <v>3</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="I13" s="10">
-        <v>2.6281983563258698E-2</v>
-      </c>
-      <c r="J13" s="10">
-        <v>1.0241367853735699</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="11">
+        <v>1.70897489233542E-2</v>
+      </c>
+      <c r="J13" s="10"/>
       <c r="K13" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D14" s="5">
         <v>1E-3</v>
@@ -1371,35 +1378,35 @@
       <c r="G14" s="5">
         <v>3</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>51</v>
+      <c r="H14" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="I14" s="10">
-        <v>2.4048869840342501E-2</v>
+        <v>2.6281983563258698E-2</v>
       </c>
       <c r="J14" s="10">
-        <v>1.01567187527867</v>
+        <v>1.0241367853735699</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D15" s="5">
         <v>1E-3</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="F15" s="5">
         <v>100</v>
@@ -1408,28 +1415,28 @@
         <v>3</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="I15" s="11">
-        <v>2.3460846365785701E-2</v>
+        <v>51</v>
+      </c>
+      <c r="I15" s="10">
+        <v>2.4048869840342501E-2</v>
       </c>
       <c r="J15" s="10">
-        <v>1.0139060054064699</v>
+        <v>1.01567187527867</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D16" s="5">
         <v>1E-3</v>
@@ -1441,37 +1448,37 @@
         <v>100</v>
       </c>
       <c r="G16" s="5">
-        <v>4</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="I16" s="10">
-        <v>1.1261041047572499E-2</v>
+        <v>3</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="11">
+        <v>2.3460846365785701E-2</v>
       </c>
       <c r="J16" s="10">
-        <v>1.03511575669834</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1.0139060054064699</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="D17" s="5">
         <v>1E-3</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="F17" s="5">
         <v>100</v>
@@ -1479,35 +1486,35 @@
       <c r="G17" s="5">
         <v>4</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>58</v>
+      <c r="H17" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="I17" s="10">
-        <v>2.3904601278544602E-2</v>
+        <v>1.1261041047572499E-2</v>
       </c>
       <c r="J17" s="10">
-        <v>1.01366590838736</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1.03511575669834</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="5">
         <v>1E-3</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F18" s="5">
         <v>100</v>
@@ -1516,28 +1523,28 @@
         <v>4</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I18" s="10">
-        <v>2.32061401095221E-2</v>
+        <v>2.3904601278544602E-2</v>
       </c>
       <c r="J18" s="10">
-        <v>1.0065377628882399</v>
+        <v>1.01366590838736</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D19" s="5">
         <v>1E-3</v>
@@ -1552,25 +1559,25 @@
         <v>4</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I19" s="10">
-        <v>1.0682632046597499E-2</v>
+        <v>2.32061401095221E-2</v>
       </c>
       <c r="J19" s="10">
-        <v>1.02675945497015</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>1.0065377628882399</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>61</v>
@@ -1579,7 +1586,7 @@
         <v>1E-3</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="F20" s="5">
         <v>100</v>
@@ -1587,29 +1594,29 @@
       <c r="G20" s="5">
         <v>4</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="I20" s="11">
-        <v>1.0635255409829399E-2</v>
+      <c r="H20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1.0682632046597499E-2</v>
       </c>
       <c r="J20" s="10">
-        <v>1.0271734113490001</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+        <v>1.02675945497015</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <f>1+A20</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D21" s="5">
         <v>1E-3</v>
@@ -1617,36 +1624,60 @@
       <c r="E21" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>70</v>
+      <c r="F21" s="5">
+        <v>100</v>
       </c>
       <c r="G21" s="5">
         <v>4</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I21" s="11">
+        <v>1.0635255409829399E-2</v>
+      </c>
+      <c r="J21" s="10">
+        <v>1.0271734113490001</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="5">
+        <v>4</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I22" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J22" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K22" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -1662,9 +1693,6 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1675,12 +1703,12 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="12"/>
+      <c r="B25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1690,19 +1718,34 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" s="14"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="2"/>
+    <row r="26" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>